<commit_message>
Latest fixes and providing propper errro msg
</commit_message>
<xml_diff>
--- a/testCase/CommissionSystemTestCases.xlsx
+++ b/testCase/CommissionSystemTestCases.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\GUI-Testing\testCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B29BAE-FA0F-4448-BEB2-90113971B579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482922C9-960E-4686-A240-8A9551A6937F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F239CE29-EF98-4C31-AD33-9259465996C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Logout" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
   <si>
     <t>type</t>
   </si>
@@ -101,16 +102,34 @@
     <t xml:space="preserve">Not able to login </t>
   </si>
   <si>
-    <t>TC 01:01 - Login Test 1</t>
-  </si>
-  <si>
-    <t>TC 01:02 - Login Test 2</t>
-  </si>
-  <si>
     <t>data/Test Title</t>
   </si>
   <si>
-    <t>admin12</t>
+    <t>TC 02:01 - Logout</t>
+  </si>
+  <si>
+    <t>//*[@id="root"]/div/div/div[2]/header/div[2]/ul/li[2]/div/a</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//*[@id="root"]/div/div/div[2]/header/div[2]/ul/li[2]/div/div/a[2]</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>stArt</t>
+  </si>
+  <si>
+    <t>enD</t>
+  </si>
+  <si>
+    <t>TC : 01</t>
+  </si>
+  <si>
+    <t>TC : 02</t>
   </si>
 </sst>
 </file>
@@ -474,7 +493,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +518,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
         <v>13</v>
@@ -512,77 +531,66 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -590,24 +598,35 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="G8" t="s">
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -620,7 +639,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -668,7 +687,7 @@
         <v>17</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -687,99 +706,130 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" t="s">
-        <v>21</v>
-      </c>
+      <c r="A20" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D91AF6-398F-44BE-B023-C473864AF5DB}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="61.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>